<commit_message>
Update -> 'Diretor' = Gestor Direto
</commit_message>
<xml_diff>
--- a/formularioProject/planilhas/SOLICITAÇÕES.xlsx
+++ b/formularioProject/planilhas/SOLICITAÇÕES.xlsx
@@ -509,7 +509,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L3" sqref="A2:L3"/>
@@ -713,6 +713,66 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>45439</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Thayna Silva Santana</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Rua Castro Alves</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>thayna.silva</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Francisco</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Estagiario</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Automação</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Todos</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Notebook + Carregador</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>LUM-001-001-012</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Mayara Almeilda</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>23/05/2024 16:20:15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add required e placeholders em todos fields
</commit_message>
<xml_diff>
--- a/formularioProject/planilhas/SOLICITAÇÕES.xlsx
+++ b/formularioProject/planilhas/SOLICITAÇÕES.xlsx
@@ -509,7 +509,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L3" sqref="A2:L3"/>
@@ -773,6 +773,66 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="7" t="n">
+        <v>45439</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Thayna Silva Santana</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Aristides Attico 2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>thayna.santana</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Francisco</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Estagiaria</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Automação</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Todos</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Notebook + Carregador</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>LUM-001-001-078</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Mayara Almeida</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>23/05/2024 17:46:56</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>